<commit_message>
changed code for script
</commit_message>
<xml_diff>
--- a/Resources/GoogleMapTestData.xlsx
+++ b/Resources/GoogleMapTestData.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\AppiumFramework\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gyanadeep Sahoo\eclipse-workspace\AppiumFramework\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2DC5E4-643E-40EB-B26F-31B8B92D1751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEA8492-9F34-4A19-96EC-8243D0F29C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{273AC0EA-EF08-44F8-A0C8-9FE87C213ADF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{273AC0EA-EF08-44F8-A0C8-9FE87C213ADF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="76">
   <si>
     <t>KeyWord</t>
   </si>
@@ -184,37 +185,76 @@
     <t>Roofers</t>
   </si>
   <si>
+    <t>https://roofer-peabodyma.com/commercial-roofing/</t>
+  </si>
+  <si>
+    <t>https://roofer-peabodyma.com/roof-replacement/</t>
+  </si>
+  <si>
+    <t>https://roofer-peabodyma.com/roof-repair/</t>
+  </si>
+  <si>
+    <t>Roofing Contractor</t>
+  </si>
+  <si>
+    <t>Point-A_Latitude</t>
+  </si>
+  <si>
+    <t>Point-A_Langitude</t>
+  </si>
+  <si>
+    <t>Point-B_Latitude</t>
+  </si>
+  <si>
+    <t>Point-A_Longitude</t>
+  </si>
+  <si>
+    <t>Point-B_Longitude</t>
+  </si>
+  <si>
+    <t>https://mackmediagroup.com/video-production-ct/political-campaign-videos/</t>
+  </si>
+  <si>
+    <t>Massage near me</t>
+  </si>
+  <si>
+    <t>Best spa</t>
+  </si>
+  <si>
+    <t>Best massage</t>
+  </si>
+  <si>
+    <t>Peony SPA</t>
+  </si>
+  <si>
+    <t>Digital marketing agency</t>
+  </si>
+  <si>
+    <t>Best massage near me</t>
+  </si>
+  <si>
+    <t>Spa near me</t>
+  </si>
+  <si>
+    <t>Massage in orange</t>
+  </si>
+  <si>
+    <t>Best massage in orange</t>
+  </si>
+  <si>
+    <t>Spa in Orange</t>
+  </si>
+  <si>
+    <t>https://mackmediagroup.com/video-production-ct/corporate-video-production/</t>
+  </si>
+  <si>
     <t>https://roofer-peabodyma.com/residential-roofing/</t>
   </si>
   <si>
-    <t>https://roofer-peabodyma.com/commercial-roofing/</t>
-  </si>
-  <si>
-    <t>https://roofer-peabodyma.com/roof-replacement/</t>
-  </si>
-  <si>
-    <t>https://roofer-peabodyma.com/roof-repair/</t>
-  </si>
-  <si>
-    <t>https://roofer-peabodyma.com/blogs/</t>
-  </si>
-  <si>
-    <t>Roofing Contractor</t>
-  </si>
-  <si>
-    <t>Point-A_Latitude</t>
-  </si>
-  <si>
-    <t>Point-A_Langitude</t>
-  </si>
-  <si>
-    <t>Point-B_Latitude</t>
-  </si>
-  <si>
-    <t>Point-A_Longitude</t>
-  </si>
-  <si>
-    <t>Point-B_Longitude</t>
+    <t>Landing Page1</t>
+  </si>
+  <si>
+    <t>Landing Page 2</t>
   </si>
 </sst>
 </file>
@@ -279,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -289,6 +329,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -604,42 +649,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312EE4C8-5289-49BF-982C-6C412A325477}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="60.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="64.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="55.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="55.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -672,7 +717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>41.4639528175518</v>
       </c>
@@ -713,7 +758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>25.838990632130599</v>
       </c>
@@ -751,7 +796,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>41.772137772053398</v>
       </c>
@@ -792,7 +837,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>41.185062176543298</v>
       </c>
@@ -836,7 +881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>41.185062176543298</v>
       </c>
@@ -880,7 +925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>41.185062176543298</v>
       </c>
@@ -924,7 +969,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>41.185062176543298</v>
       </c>
@@ -968,7 +1013,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>41.185062176543298</v>
       </c>
@@ -1012,7 +1057,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>41.185062176543298</v>
       </c>
@@ -1056,7 +1101,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>41.772137772053398</v>
       </c>
@@ -1097,7 +1142,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>41.772137772053398</v>
       </c>
@@ -1138,7 +1183,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>41.772137772053398</v>
       </c>
@@ -1179,7 +1224,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>41.772137772053398</v>
       </c>
@@ -1220,7 +1265,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>41.772137772053398</v>
       </c>
@@ -1261,7 +1306,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>41.4639528175518</v>
       </c>
@@ -1302,7 +1347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>41.4639528175518</v>
       </c>
@@ -1343,7 +1388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>41.4639528175518</v>
       </c>
@@ -1384,7 +1429,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>41.4639528175518</v>
       </c>
@@ -1425,7 +1470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>40.801805195325699</v>
       </c>
@@ -1467,6 +1512,297 @@
       </c>
       <c r="N20" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>41.2554995886372</v>
+      </c>
+      <c r="B24">
+        <v>-73.016931795998303</v>
+      </c>
+      <c r="C24">
+        <v>41.248796273874198</v>
+      </c>
+      <c r="D24">
+        <v>-73.024373234163207</v>
+      </c>
+      <c r="E24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>41.2554995886372</v>
+      </c>
+      <c r="B25">
+        <v>-73.016931795998303</v>
+      </c>
+      <c r="C25">
+        <v>41.248796273874198</v>
+      </c>
+      <c r="D25">
+        <v>-73.024373234163207</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>41.2554995886372</v>
+      </c>
+      <c r="B26">
+        <v>-73.016931795998303</v>
+      </c>
+      <c r="C26">
+        <v>41.248796273874198</v>
+      </c>
+      <c r="D26">
+        <v>-73.024373234163207</v>
+      </c>
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26">
+        <v>26</v>
+      </c>
+      <c r="G26" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>41.2554995886372</v>
+      </c>
+      <c r="B27">
+        <v>-73.016931795998303</v>
+      </c>
+      <c r="C27">
+        <v>41.248796273874198</v>
+      </c>
+      <c r="D27">
+        <v>-73.024373234163207</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>41.2554995886372</v>
+      </c>
+      <c r="B28">
+        <v>-73.016931795998303</v>
+      </c>
+      <c r="C28">
+        <v>41.248796273874198</v>
+      </c>
+      <c r="D28">
+        <v>-73.024373234163207</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>41.2554995886372</v>
+      </c>
+      <c r="B29">
+        <v>-73.016931795998303</v>
+      </c>
+      <c r="C29">
+        <v>41.248796273874198</v>
+      </c>
+      <c r="D29">
+        <v>-73.024373234163207</v>
+      </c>
+      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>41.2554995886372</v>
+      </c>
+      <c r="B30">
+        <v>-73.016931795998303</v>
+      </c>
+      <c r="C30">
+        <v>41.248796273874198</v>
+      </c>
+      <c r="D30">
+        <v>-73.024373234163207</v>
+      </c>
+      <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30">
+        <v>23</v>
+      </c>
+      <c r="G30" t="s">
+        <v>65</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>41.2554995886372</v>
+      </c>
+      <c r="B31">
+        <v>-73.016931795998303</v>
+      </c>
+      <c r="C31">
+        <v>41.248796273874198</v>
+      </c>
+      <c r="D31">
+        <v>-73.024373234163207</v>
+      </c>
+      <c r="E31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31">
+        <v>26</v>
+      </c>
+      <c r="G31" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>41.2554995886372</v>
+      </c>
+      <c r="B32">
+        <v>-73.016931795998303</v>
+      </c>
+      <c r="C32">
+        <v>41.248796273874198</v>
+      </c>
+      <c r="D32">
+        <v>-73.024373234163207</v>
+      </c>
+      <c r="E32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32">
+        <v>26</v>
+      </c>
+      <c r="G32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>41.2554995886372</v>
+      </c>
+      <c r="B33">
+        <v>-73.016931795998303</v>
+      </c>
+      <c r="C33">
+        <v>41.248796273874198</v>
+      </c>
+      <c r="D33">
+        <v>-73.024373234163207</v>
+      </c>
+      <c r="E33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
+        <v>65</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1482,41 +1818,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEACE24-A917-49D1-A3DA-B7C71F9500C7}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="76.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -1534,10 +1870,10 @@
         <v>4</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>7</v>
@@ -1549,18 +1885,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>42.564126000000002</v>
+        <v>42.545376829821798</v>
       </c>
       <c r="B2">
-        <v>-71.026185999999996</v>
+        <v>-70.986441357769294</v>
       </c>
       <c r="C2">
-        <v>42.518720999999999</v>
+        <v>42.5400490472963</v>
       </c>
       <c r="D2">
-        <v>-70.939668999999995</v>
+        <v>-70.988479836650498</v>
       </c>
       <c r="E2" t="s">
         <v>51</v>
@@ -1577,98 +1913,346 @@
       <c r="I2">
         <v>40</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>52</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>25.810867644825901</v>
+      </c>
+      <c r="B3">
+        <v>-80.329834441935404</v>
+      </c>
+      <c r="C3">
+        <v>25.801876422524298</v>
+      </c>
+      <c r="D3">
+        <v>-80.3299042828193</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>45</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>42.545376829821798</v>
+      </c>
+      <c r="B4">
+        <v>-70.986441357769294</v>
+      </c>
+      <c r="C4">
+        <v>42.5400490472963</v>
+      </c>
+      <c r="D4">
+        <v>-70.988479836650498</v>
+      </c>
+      <c r="E4" t="s">
         <v>55</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>42.562735000000004</v>
-      </c>
-      <c r="B3">
-        <v>-71.024298000000002</v>
-      </c>
-      <c r="C3">
-        <v>42.522643000000002</v>
-      </c>
-      <c r="D3">
-        <v>-70.946191999999996</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3">
+      <c r="F4">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>50</v>
       </c>
-      <c r="H3">
+      <c r="H4">
         <v>30</v>
       </c>
-      <c r="I3">
+      <c r="I4">
         <v>50</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="J4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>56</v>
-      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J7" s="2"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="K13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="K15" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{1249EB21-8FE5-47A9-ABEC-C5F196470360}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{CD0FC2F5-8940-4C65-906A-B99EE5745F6E}"/>
-    <hyperlink ref="M3" r:id="rId3" xr:uid="{DA636DCD-123F-40BF-BC56-572284F656CB}"/>
-    <hyperlink ref="M2" r:id="rId4" xr:uid="{2E6EAD24-FE0A-4A20-837F-C0A07C688BA6}"/>
-    <hyperlink ref="L2" r:id="rId5" xr:uid="{307AFF06-D7B3-4071-ADD7-2C353382C5C5}"/>
-    <hyperlink ref="N3" r:id="rId6" xr:uid="{1C6A19AA-D855-470C-AFF1-3C5557529897}"/>
-    <hyperlink ref="J3" r:id="rId7" xr:uid="{127E39B6-9E76-4C73-B912-A5872FAC4766}"/>
-    <hyperlink ref="N2" r:id="rId8" xr:uid="{394531C1-B141-41D1-B811-18E2B8F6374F}"/>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{24D88E43-011C-4968-8DDF-B77139F29FD7}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{542A77C7-9179-452E-A939-0BC8618A540E}"/>
+    <hyperlink ref="K2" r:id="rId3" xr:uid="{0CA56FBF-7ECF-4011-9FCD-D6E66FEBBFE4}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{7A066B5B-0C0E-4B38-95ED-D94215180711}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B781C995-CC2C-430E-96C5-09097A148788}">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="74.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="76.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>42.545376829821798</v>
+      </c>
+      <c r="B2">
+        <v>-70.986441357769294</v>
+      </c>
+      <c r="C2">
+        <v>42.5400490472963</v>
+      </c>
+      <c r="D2">
+        <v>-70.988479836650498</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>25.810867644825901</v>
+      </c>
+      <c r="B3">
+        <v>-80.329834441935404</v>
+      </c>
+      <c r="C3">
+        <v>25.801876422524298</v>
+      </c>
+      <c r="D3">
+        <v>-80.3299042828193</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>45</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>42.545376829821798</v>
+      </c>
+      <c r="B4">
+        <v>-70.986441357769294</v>
+      </c>
+      <c r="C4">
+        <v>42.5400490472963</v>
+      </c>
+      <c r="D4">
+        <v>-70.988479836650498</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{3639D716-7BA4-44CF-999B-81EDEFB6F231}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{4CC86150-053B-4281-8FA0-F9D95F25BAEA}"/>
+    <hyperlink ref="K2" r:id="rId3" xr:uid="{70328AF4-B5CC-4FAC-A29F-74C2518BA94D}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{0188B5D9-5416-4BD9-BDA1-3393F3C3D4FE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D2E4D9AF2DEF4498DEBE42431EB34A7" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1d270922d44a5b78717a4b147e11fd86">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="21290b85-8e0e-4544-9b54-65ec2ea8aad1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="878ba3062844f1f5d19274d61335c757" ns3:_="">
     <xsd:import namespace="21290b85-8e0e-4544-9b54-65ec2ea8aad1"/>
@@ -1806,31 +2390,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55C74F9F-E0D3-4BAB-88E8-2452B26F1F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="21290b85-8e0e-4544-9b54-65ec2ea8aad1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A36AE763-E731-4E22-A2A8-B95A3FB1C3CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{460A2550-ADB4-46BE-921E-EAECDA3B84E5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1846,4 +2421,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A36AE763-E731-4E22-A2A8-B95A3FB1C3CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55C74F9F-E0D3-4BAB-88E8-2452B26F1F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="21290b85-8e0e-4544-9b54-65ec2ea8aad1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>